<commit_message>
lab 7 low pass
</commit_message>
<xml_diff>
--- a/lab07/data.xlsx
+++ b/lab07/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twes1\Documents\RIT_fall_2023\CMPE460\cmpe460-reports\lab07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD5A014-BB95-4786-85BC-F99F0675839B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFF1BA3-1514-46D7-8714-8C472C214848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{463FAFBF-88EB-4DA5-B26E-A8F1F6E7E00C}"/>
+    <workbookView xWindow="-78" yWindow="0" windowWidth="11676" windowHeight="12318" xr2:uid="{463FAFBF-88EB-4DA5-B26E-A8F1F6E7E00C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Calculated Vout</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>PART8</t>
+  </si>
+  <si>
+    <t>amplitude in</t>
+  </si>
+  <si>
+    <t>amplitude out</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C69C5EF-552B-46AC-808B-AC08B3B6E7E6}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -465,6 +471,8 @@
     <col min="2" max="2" width="17.20703125" customWidth="1"/>
     <col min="3" max="3" width="16.83984375" customWidth="1"/>
     <col min="4" max="4" width="16.41796875" customWidth="1"/>
+    <col min="6" max="6" width="11.1015625" customWidth="1"/>
+    <col min="7" max="7" width="11.9453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -786,7 +794,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>0.6</v>
       </c>
@@ -798,7 +806,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>0.8</v>
       </c>
@@ -810,7 +818,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>1</v>
       </c>
@@ -822,12 +830,12 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -841,7 +849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>0</v>
       </c>
@@ -856,7 +864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>1</v>
       </c>
@@ -871,7 +879,7 @@
         <v>-0.99</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>1</v>
       </c>
@@ -886,7 +894,7 @@
         <v>-1.99</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>-1</v>
       </c>
@@ -901,7 +909,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>3</v>
       </c>
@@ -916,7 +924,7 @@
         <v>-4.99</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>-2</v>
       </c>
@@ -931,7 +939,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>1</v>
       </c>
@@ -946,12 +954,12 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -964,63 +972,239 @@
       <c r="D48" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49">
+        <f>G49/F49</f>
+        <v>2.2285714285714286</v>
+      </c>
+      <c r="C49">
+        <f>20*LOG(G49/F49,10)</f>
+        <v>6.9605311668040946</v>
+      </c>
+      <c r="D49">
+        <v>5.7</v>
+      </c>
+      <c r="F49">
+        <v>3.5</v>
+      </c>
+      <c r="G49">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>500</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50">
+        <f t="shared" ref="B50:B58" si="5">G50/F50</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:C58" si="6">20*LOG(G50/F50,10)</f>
+        <v>6.7158420384638617</v>
+      </c>
+      <c r="D50">
+        <v>5.5</v>
+      </c>
+      <c r="F50">
+        <v>3.6</v>
+      </c>
+      <c r="G50">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>5000</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51">
+        <f t="shared" si="5"/>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="6"/>
+        <v>6.3751752524882557</v>
+      </c>
+      <c r="D51">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>3.6</v>
+      </c>
+      <c r="G51">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>10000</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52">
+        <f t="shared" si="5"/>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="6"/>
+        <v>6.3751752524882557</v>
+      </c>
+      <c r="D52">
+        <v>13.5</v>
+      </c>
+      <c r="F52">
+        <v>3.6</v>
+      </c>
+      <c r="G52">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>50000</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53">
+        <f t="shared" si="5"/>
+        <v>1.8</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="6"/>
+        <v>5.1054501020661212</v>
+      </c>
+      <c r="D53">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="F53">
+        <v>3.5</v>
+      </c>
+      <c r="G53">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>80000</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54">
+        <f t="shared" si="5"/>
+        <v>1.0285714285714287</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="6"/>
+        <v>0.2446891283402336</v>
+      </c>
+      <c r="D54">
+        <v>175.4</v>
+      </c>
+      <c r="F54">
+        <v>3.5</v>
+      </c>
+      <c r="G54">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>100000</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55">
+        <f t="shared" si="5"/>
+        <v>0.82857142857142851</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="6"/>
+        <v>-1.6334009290263916</v>
+      </c>
+      <c r="D55">
+        <v>177.7</v>
+      </c>
+      <c r="F55">
+        <v>3.5</v>
+      </c>
+      <c r="G55">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>200000</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56">
+        <f t="shared" si="5"/>
+        <v>0.31428571428571433</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="6"/>
+        <v>-10.05350718384101</v>
+      </c>
+      <c r="D56">
+        <v>-169</v>
+      </c>
+      <c r="F56">
+        <v>3.5</v>
+      </c>
+      <c r="G56">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>300000</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57">
+        <f t="shared" si="5"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="6"/>
+        <v>-16.901960800285135</v>
+      </c>
+      <c r="D57">
+        <v>-154.69999999999999</v>
+      </c>
+      <c r="F57">
+        <v>3.5</v>
+      </c>
+      <c r="G57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>500000</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58">
+        <f t="shared" si="5"/>
+        <v>5.7142857142857148E-2</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="6"/>
+        <v>-24.860760973725885</v>
+      </c>
+      <c r="D58">
+        <v>-123</v>
+      </c>
+      <c r="F58">
+        <v>3.5</v>
+      </c>
+      <c r="G58">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -1034,17 +1218,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>500</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>5000</v>
       </c>

</xml_diff>

<commit_message>
added graphs for low pass data
</commit_message>
<xml_diff>
--- a/lab07/data.xlsx
+++ b/lab07/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twes1\Documents\RIT_fall_2023\CMPE460\cmpe460-reports\lab07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFF1BA3-1514-46D7-8714-8C472C214848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4241FF-C7F7-4320-81AB-44964403DEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="11676" windowHeight="12318" xr2:uid="{463FAFBF-88EB-4DA5-B26E-A8F1F6E7E00C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{463FAFBF-88EB-4DA5-B26E-A8F1F6E7E00C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,6 +163,1934 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>gain</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (dB) vs frequency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$49:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$49:$C$58</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.9605311668040946</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7158420384638617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3751752524882557</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3751752524882557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1054501020661212</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2446891283402336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.6334009290263916</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.05350718384101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-16.901960800285135</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-24.860760973725885</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25A0-430F-9F01-DE815E5444B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1624083471"/>
+        <c:axId val="1625479887"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1624083471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1625479887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1625479887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1624083471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>phase vs frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$49:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$49:$E$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>175.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>177.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>205.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA5A-4701-8B91-1D6A8D36A642}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1624115151"/>
+        <c:axId val="1789332815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1624115151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1789332815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1789332815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1624115151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>344532</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>138520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>433795</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>138520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{385B5C84-3D18-E584-D2E2-9035C33A723D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>41364</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>75927</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>132804</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>75927</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C60E300A-B9CD-4E09-1772-B4B5A9B82467}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -462,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C69C5EF-552B-46AC-808B-AC08B3B6E7E6}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -987,11 +2915,14 @@
         <f>G49/F49</f>
         <v>2.2285714285714286</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="3">
         <f>20*LOG(G49/F49,10)</f>
         <v>6.9605311668040946</v>
       </c>
       <c r="D49">
+        <v>5.7</v>
+      </c>
+      <c r="E49">
         <v>5.7</v>
       </c>
       <c r="F49">
@@ -1009,11 +2940,14 @@
         <f t="shared" ref="B50:B58" si="5">G50/F50</f>
         <v>2.1666666666666665</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="3">
         <f t="shared" ref="C50:C58" si="6">20*LOG(G50/F50,10)</f>
         <v>6.7158420384638617</v>
       </c>
       <c r="D50">
+        <v>5.5</v>
+      </c>
+      <c r="E50">
         <v>5.5</v>
       </c>
       <c r="F50">
@@ -1031,11 +2965,14 @@
         <f t="shared" si="5"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="3">
         <f t="shared" si="6"/>
         <v>6.3751752524882557</v>
       </c>
       <c r="D51">
+        <v>9</v>
+      </c>
+      <c r="E51">
         <v>9</v>
       </c>
       <c r="F51">
@@ -1053,11 +2990,14 @@
         <f t="shared" si="5"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
         <f t="shared" si="6"/>
         <v>6.3751752524882557</v>
       </c>
       <c r="D52">
+        <v>13.5</v>
+      </c>
+      <c r="E52">
         <v>13.5</v>
       </c>
       <c r="F52">
@@ -1075,11 +3015,14 @@
         <f t="shared" si="5"/>
         <v>1.8</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="3">
         <f t="shared" si="6"/>
         <v>5.1054501020661212</v>
       </c>
       <c r="D53">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="E53">
         <v>148.19999999999999</v>
       </c>
       <c r="F53">
@@ -1097,11 +3040,14 @@
         <f t="shared" si="5"/>
         <v>1.0285714285714287</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="3">
         <f t="shared" si="6"/>
         <v>0.2446891283402336</v>
       </c>
       <c r="D54">
+        <v>175.4</v>
+      </c>
+      <c r="E54">
         <v>175.4</v>
       </c>
       <c r="F54">
@@ -1119,11 +3065,14 @@
         <f t="shared" si="5"/>
         <v>0.82857142857142851</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="3">
         <f t="shared" si="6"/>
         <v>-1.6334009290263916</v>
       </c>
       <c r="D55">
+        <v>177.7</v>
+      </c>
+      <c r="E55">
         <v>177.7</v>
       </c>
       <c r="F55">
@@ -1141,12 +3090,16 @@
         <f t="shared" si="5"/>
         <v>0.31428571428571433</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="3">
         <f t="shared" si="6"/>
         <v>-10.05350718384101</v>
       </c>
       <c r="D56">
         <v>-169</v>
+      </c>
+      <c r="E56">
+        <f>D56+360</f>
+        <v>191</v>
       </c>
       <c r="F56">
         <v>3.5</v>
@@ -1163,12 +3116,16 @@
         <f t="shared" si="5"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="3">
         <f t="shared" si="6"/>
         <v>-16.901960800285135</v>
       </c>
       <c r="D57">
         <v>-154.69999999999999</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:E58" si="7">D57+360</f>
+        <v>205.3</v>
       </c>
       <c r="F57">
         <v>3.5</v>
@@ -1185,12 +3142,16 @@
         <f t="shared" si="5"/>
         <v>5.7142857142857148E-2</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="3">
         <f t="shared" si="6"/>
         <v>-24.860760973725885</v>
       </c>
       <c r="D58">
         <v>-123</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="7"/>
+        <v>237</v>
       </c>
       <c r="F58">
         <v>3.5</v>
@@ -1329,5 +3290,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>